<commit_message>
add new testcases and add new script in selenium code
</commit_message>
<xml_diff>
--- a/01_Test_Case_Development/TestCaseDevelopment.xlsx
+++ b/01_Test_Case_Development/TestCaseDevelopment.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91931\Desktop\Netflix_WebApp_Automation\01_Test_Case_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BFE08A-76CA-4538-A947-4848A32C71DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB291300-0DF1-4D11-A162-84536AE9316B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="94">
   <si>
     <t>Created By</t>
   </si>
@@ -257,6 +258,69 @@
   </si>
   <si>
     <t>Verify Login With Valid Credentials in different browser</t>
+  </si>
+  <si>
+    <t>TCL008</t>
+  </si>
+  <si>
+    <t>TCL009</t>
+  </si>
+  <si>
+    <t>TCL010</t>
+  </si>
+  <si>
+    <t>TCL011</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Verify successful logout redirects the user to the login page</t>
+  </si>
+  <si>
+    <t>Verify that the session is terminated after logout</t>
+  </si>
+  <si>
+    <t>Verify logout functionality in different browsers (cross-browser testing)</t>
+  </si>
+  <si>
+    <t>Verify logout functionality when the internet connection is lost during the process</t>
+  </si>
+  <si>
+    <t>User account credentials</t>
+  </si>
+  <si>
+    <t>1. Navigate to the account/logout option.
+2. Click on the logout button</t>
+  </si>
+  <si>
+    <t>1. Logout from the account.
+2. Attempt to navigate back using the browser's back button.</t>
+  </si>
+  <si>
+    <t>1. Disconnect the internet connection.
+2. Attempt to log out.
+3. Reconnect the internet.</t>
+  </si>
+  <si>
+    <t>1. Open Netflix in Chrome and Edge.
+2. Login to the account.
+3. Perform logout action.</t>
+  </si>
+  <si>
+    <t>1. User is logged in</t>
+  </si>
+  <si>
+    <t>User is redirected to the login page.</t>
+  </si>
+  <si>
+    <t>User remains on the login page, and no previous session data is accessible.</t>
+  </si>
+  <si>
+    <t>System displays an error message or logs out automatically after reconnection</t>
+  </si>
+  <si>
+    <t>Logout should function seamlessly on both browsers, redirecting to the login page.</t>
   </si>
 </sst>
 </file>
@@ -364,44 +428,44 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -457,7 +521,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DD051A1-F5AF-4E0C-9B05-8FE6170F8E39}" name="Table3" displayName="Table3" ref="A12:E20" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DD051A1-F5AF-4E0C-9B05-8FE6170F8E39}" name="Table3" displayName="Table3" ref="A12:E21" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{298EAB1B-CE47-48B1-B114-A849A5E4FBC3}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{57FEDC33-0ABF-4C2A-85EA-404A55DAE3A2}" name="Column2" dataDxfId="12"/>
@@ -470,16 +534,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6A09C3-FC34-4D8C-A5D4-8072AD62C9CC}" name="Table1" displayName="Table1" ref="A3:J9" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6A09C3-FC34-4D8C-A5D4-8072AD62C9CC}" name="Table1" displayName="Table1" ref="A3:J12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{FA4190CF-869B-4AAD-AB85-D1D406A51822}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{0311160A-A013-418B-9B3E-7E1B2ADD899B}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{AD8808FF-8F1D-4CC3-B622-EFC81FB03BD4}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{9C5B5206-F216-4894-9B82-02A62D750777}" name="Column4" headerRowDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{82A966FE-4084-4D7C-963B-761EEE522C1D}" name="Column5" headerRowDxfId="1" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{37CB4985-744D-4D93-A860-52EF4AABD929}" name="Column6" headerRowDxfId="2" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{C9BD0B30-409A-4BBC-B40E-4748725B9EDC}" name="Column7" headerRowDxfId="3" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{FD7333FE-2577-49E7-9EEB-639591C024D9}" name="Column8" headerRowDxfId="4" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{9C5B5206-F216-4894-9B82-02A62D750777}" name="Column4" headerRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{82A966FE-4084-4D7C-963B-761EEE522C1D}" name="Column5" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{37CB4985-744D-4D93-A860-52EF4AABD929}" name="Column6" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{C9BD0B30-409A-4BBC-B40E-4748725B9EDC}" name="Column7" headerRowDxfId="3" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{FD7333FE-2577-49E7-9EEB-639591C024D9}" name="Column8" headerRowDxfId="2" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{FFBE56F5-BD1B-45B6-82E9-4F8E26DCAC44}" name="Column9"/>
     <tableColumn id="10" xr3:uid="{6A548CC8-DC51-4A5D-B5CC-BC1FD564AB3A}" name="Column10"/>
   </tableColumns>
@@ -750,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,10 +831,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -844,6 +908,9 @@
       <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
@@ -858,6 +925,9 @@
       <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
@@ -929,15 +999,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>20</v>
@@ -951,13 +1021,13 @@
         <v>41</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>35</v>
       </c>
@@ -965,11 +1035,15 @@
         <v>41</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="6"/>
+      <c r="C21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -986,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726732DD-22CB-4F62-A4AF-B8D521F92FCF}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A4" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -999,8 +1073,8 @@
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6328125" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" customWidth="1"/>
+    <col min="6" max="6" width="29.08984375" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" customWidth="1"/>
     <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.1796875" customWidth="1"/>
@@ -1045,10 +1119,10 @@
       <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>63</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -1074,7 +1148,7 @@
       <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -1100,7 +1174,7 @@
       <c r="C4" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1152,7 +1226,9 @@
       <c r="C6" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="E6" s="7" t="s">
         <v>57</v>
       </c>
@@ -1218,15 +1294,109 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1235,4 +1405,16 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5EE776-2040-40E3-8C52-44FCC97D5826}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test cases for acc management and search and improve function in automation script
</commit_message>
<xml_diff>
--- a/01_Test_Case_Development/TestCaseDevelopment.xlsx
+++ b/01_Test_Case_Development/TestCaseDevelopment.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91931\Desktop\Netflix_WebApp_Automation\01_Test_Case_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB291300-0DF1-4D11-A162-84536AE9316B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6DEB04-4E06-42DA-99AE-65127E5E2C4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Login TC" sheetId="2" r:id="rId2"/>
+    <sheet name="Account Management TC" sheetId="3" r:id="rId3"/>
+    <sheet name="Search TC" sheetId="4" r:id="rId4"/>
+    <sheet name="General Navigation TC" sheetId="5" r:id="rId5"/>
+    <sheet name="PlayBack Controls Tc" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="191">
   <si>
     <t>Created By</t>
   </si>
@@ -321,13 +324,480 @@
   </si>
   <si>
     <t>Logout should function seamlessly on both browsers, redirecting to the login page.</t>
+  </si>
+  <si>
+    <t>TCAM001</t>
+  </si>
+  <si>
+    <t>TCAM002</t>
+  </si>
+  <si>
+    <t>TCAM003</t>
+  </si>
+  <si>
+    <t>TCAM004</t>
+  </si>
+  <si>
+    <t>TCAM005</t>
+  </si>
+  <si>
+    <t>TCAM006</t>
+  </si>
+  <si>
+    <t>TCAM007</t>
+  </si>
+  <si>
+    <t>TCAM008</t>
+  </si>
+  <si>
+    <t>TCAM009</t>
+  </si>
+  <si>
+    <t>TCAM010</t>
+  </si>
+  <si>
+    <t>TCAM011</t>
+  </si>
+  <si>
+    <t>TCAM012</t>
+  </si>
+  <si>
+    <t>TCAM013</t>
+  </si>
+  <si>
+    <t>Valid user data (Name, Email, Password)</t>
+  </si>
+  <si>
+    <t>Verify user profile creation</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix account management page</t>
+  </si>
+  <si>
+    <t>Profile is successfully created and visible in the list of profiles.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Profile Management" section.
+2. Click on "Create New Profile."
+3. Enter valid user data and click "Save".</t>
+  </si>
+  <si>
+    <t>Invalid data (Empty fields, special chars)</t>
+  </si>
+  <si>
+    <t>Verify error handling for invalid data</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Profile Management" section.
+2. Click on "Create New Profile."
+3. Enter invalid data and click "Save."</t>
+  </si>
+  <si>
+    <t>Error messages displayed, no profile created.</t>
+  </si>
+  <si>
+    <t>Updated valid user data</t>
+  </si>
+  <si>
+    <t>Verify user profile update functionality</t>
+  </si>
+  <si>
+    <t>At least one profile exists in the account</t>
+  </si>
+  <si>
+    <t>1. Navigate to the existing profile.
+2. Click "Edit Profile."
+3. Update valid data and save.</t>
+  </si>
+  <si>
+    <t>Profile is updated with new information.</t>
+  </si>
+  <si>
+    <t>Invalid update data</t>
+  </si>
+  <si>
+    <t>Verify error handling during profile updates</t>
+  </si>
+  <si>
+    <t>1. Navigate to the existing profile.
+2. Click "Edit Profile."
+3. Enter invalid data and save.</t>
+  </si>
+  <si>
+    <t>Error messages displayed, no changes saved.</t>
+  </si>
+  <si>
+    <t>Existing profile</t>
+  </si>
+  <si>
+    <t>Verify user profile deletion functionality</t>
+  </si>
+  <si>
+    <t>1. Navigate to the existing profile.
+2. Click "Delete Profile."
+3. Confirm the delete action in the popup window.</t>
+  </si>
+  <si>
+    <t>Profile is deleted and removed from the list of profiles.</t>
+  </si>
+  <si>
+    <t>Empty fields (No name, No email, etc.)</t>
+  </si>
+  <si>
+    <t>Verify system rejects incomplete profile creation</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Profile Management" section.
+2. Click on "Create New Profile."
+3. Leave all fields empty and click "Save."</t>
+  </si>
+  <si>
+    <t>Error message for empty fields displayed.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Profile name with special characters (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify system handles special characters in profile names</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Profile Management" section.
+2. Enter special characters in the profile name field.
+3. Click "Save."</t>
+  </si>
+  <si>
+    <t>Profile created successfully or error message if special characters are invalid.</t>
+  </si>
+  <si>
+    <t>Profile name exceeding character limit</t>
+  </si>
+  <si>
+    <t>Verify system limits profile name length</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Profile Management" section.
+2. Enter a profile name longer than allowed (e.g., 100+ characters).
+3. Click "Save."</t>
+  </si>
+  <si>
+    <t>Error message for exceeding character limit displayed.</t>
+  </si>
+  <si>
+    <t>Confirm deletion dialog box</t>
+  </si>
+  <si>
+    <t>Verify user can confirm profile deletion</t>
+  </si>
+  <si>
+    <t>1. Navigate to the profile.
+2. Click "Delete Profile."
+3. Verify if a confirmation dialog box is displayed.
+4. Confirm deletion.</t>
+  </si>
+  <si>
+    <t>Profile is deleted successfully after confirmation.</t>
+  </si>
+  <si>
+    <t>Profile ID of deleted profile</t>
+  </si>
+  <si>
+    <t>Verify profile no longer appears after deletion</t>
+  </si>
+  <si>
+    <t>1. Delete a profile.
+2. Check the list of available profiles.</t>
+  </si>
+  <si>
+    <t>The deleted profile should no longer be visible in the list.</t>
+  </si>
+  <si>
+    <t>TCAM014</t>
+  </si>
+  <si>
+    <t>TCAM015</t>
+  </si>
+  <si>
+    <t>TCAM016</t>
+  </si>
+  <si>
+    <t>New valid email address</t>
+  </si>
+  <si>
+    <t>Verify the user can update their email address</t>
+  </si>
+  <si>
+    <t>User is logged into their account settings page</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Account Settings" section.
+2. Locate the email address field.
+3. Enter a new valid email address.
+4. Click "Save" or "Update."</t>
+  </si>
+  <si>
+    <t>Email address is updated successfully and confirmation is sent to the new email.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Invalid email formats (e.g., no </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, no domain)</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify error handling for invalid email formats</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Account Settings" section.
+2. Enter an invalid email address.
+3. Click "Save" or "Update."</t>
+  </si>
+  <si>
+    <t>Error message displayed, no changes saved</t>
+  </si>
+  <si>
+    <t>New valid password (e.g., meets complexity req)</t>
+  </si>
+  <si>
+    <t>Verify the user can update their password</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Account Settings" section.
+2. Locate the password field.
+3. Enter the current password and the new password.
+4. Click "Save" or "Update."</t>
+  </si>
+  <si>
+    <t>Password is updated successfully. User can log in with the new password.</t>
+  </si>
+  <si>
+    <t>Verify error handling for weak passwords</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Weak passwords (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>12345</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Navigate to the "Account Settings" section.
+2. Enter a weak password.
+3. Click "Save" or "Update."</t>
+  </si>
+  <si>
+    <t>Error message displayed, no changes saved.</t>
+  </si>
+  <si>
+    <t>New profile picture (valid image formats)</t>
+  </si>
+  <si>
+    <t>Verify the user can update their profile picture</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Account Settings" section.
+2. Locate the profile picture field.
+3. Upload a new valid image file (e.g., .jpg, .png).
+4. Click "Save" or "Update."</t>
+  </si>
+  <si>
+    <t>Profile picture is updated successfully.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Invalid image file (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, corrupted file)</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify error handling for invalid image uploads</t>
+  </si>
+  <si>
+    <t>1. Navigate to the "Account Settings" section.
+2. Attempt to upload an invalid image file.
+3. Click "Save" or "Update."</t>
+  </si>
+  <si>
+    <t>TCS001</t>
+  </si>
+  <si>
+    <t>TCS002</t>
+  </si>
+  <si>
+    <t>TCS003</t>
+  </si>
+  <si>
+    <t>TCS004</t>
+  </si>
+  <si>
+    <t>TCS005</t>
+  </si>
+  <si>
+    <t>TCS006</t>
+  </si>
+  <si>
+    <t>TCS007</t>
+  </si>
+  <si>
+    <t>TCS008</t>
+  </si>
+  <si>
+    <t>TCS009</t>
+  </si>
+  <si>
+    <t>TCS010</t>
+  </si>
+  <si>
+    <t>TCS011</t>
+  </si>
+  <si>
+    <t>TCS012</t>
+  </si>
+  <si>
+    <t>TCS013</t>
+  </si>
+  <si>
+    <t>TCS014</t>
+  </si>
+  <si>
+    <t>TCS015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +828,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,8 +848,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -396,11 +878,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -435,11 +967,147 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -511,10 +1179,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C47E57B-2296-45A5-AA1A-337942628575}" name="Table2" displayName="Table2" ref="A3:B7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C47E57B-2296-45A5-AA1A-337942628575}" name="Table2" displayName="Table2" ref="A3:B7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="31">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{ED7C2092-802D-4D55-A444-B5C75D826FBF}" name="Column1" headerRowDxfId="15" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7EA96A78-BA0E-406E-BFCA-4C90A19F9EAB}" name="Column2" headerRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{ED7C2092-802D-4D55-A444-B5C75D826FBF}" name="Column1" headerRowDxfId="30" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{7EA96A78-BA0E-406E-BFCA-4C90A19F9EAB}" name="Column2" headerRowDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -524,8 +1192,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DD051A1-F5AF-4E0C-9B05-8FE6170F8E39}" name="Table3" displayName="Table3" ref="A12:E21" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{298EAB1B-CE47-48B1-B114-A849A5E4FBC3}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{57FEDC33-0ABF-4C2A-85EA-404A55DAE3A2}" name="Column2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{7A3F631E-F0E8-4AAA-9860-670D033DF9BD}" name="Column3" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{57FEDC33-0ABF-4C2A-85EA-404A55DAE3A2}" name="Column2" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{7A3F631E-F0E8-4AAA-9860-670D033DF9BD}" name="Column3" dataDxfId="26"/>
     <tableColumn id="4" xr3:uid="{33C87811-FC0A-4F1E-906D-96F3E0410E43}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{D88CF226-9216-4B0E-9F96-5BA54F5B07B3}" name="Column5"/>
   </tableColumns>
@@ -534,18 +1202,78 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6A09C3-FC34-4D8C-A5D4-8072AD62C9CC}" name="Table1" displayName="Table1" ref="A3:J12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6A09C3-FC34-4D8C-A5D4-8072AD62C9CC}" name="Table1" displayName="Table1" ref="A3:J12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{FA4190CF-869B-4AAD-AB85-D1D406A51822}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{0311160A-A013-418B-9B3E-7E1B2ADD899B}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{AD8808FF-8F1D-4CC3-B622-EFC81FB03BD4}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{9C5B5206-F216-4894-9B82-02A62D750777}" name="Column4" headerRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{82A966FE-4084-4D7C-963B-761EEE522C1D}" name="Column5" headerRowDxfId="7" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{37CB4985-744D-4D93-A860-52EF4AABD929}" name="Column6" headerRowDxfId="5" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{C9BD0B30-409A-4BBC-B40E-4748725B9EDC}" name="Column7" headerRowDxfId="3" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{FD7333FE-2577-49E7-9EEB-639591C024D9}" name="Column8" headerRowDxfId="2" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{9C5B5206-F216-4894-9B82-02A62D750777}" name="Column4" headerRowDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{82A966FE-4084-4D7C-963B-761EEE522C1D}" name="Column5" headerRowDxfId="22" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{37CB4985-744D-4D93-A860-52EF4AABD929}" name="Column6" headerRowDxfId="20" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{C9BD0B30-409A-4BBC-B40E-4748725B9EDC}" name="Column7" headerRowDxfId="18" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{FD7333FE-2577-49E7-9EEB-639591C024D9}" name="Column8" headerRowDxfId="16" dataDxfId="15"/>
     <tableColumn id="9" xr3:uid="{FFBE56F5-BD1B-45B6-82E9-4F8E26DCAC44}" name="Column9"/>
     <tableColumn id="10" xr3:uid="{6A548CC8-DC51-4A5D-B5CC-BC1FD564AB3A}" name="Column10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{68C63221-97A0-4792-887D-F663C0F6D441}" name="Table5" displayName="Table5" ref="A1:J17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="14">
+  <autoFilter ref="A1:J17" xr:uid="{1824CCDB-4630-4D24-B722-9D28F2EBE92F}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{6D6A53C9-CB2B-42B5-8A0C-459649608A20}" name="Test Scenario TID"/>
+    <tableColumn id="2" xr3:uid="{2062CCCD-C2CB-4254-A6CC-757B0FC707B8}" name="Test Scenario"/>
+    <tableColumn id="3" xr3:uid="{8F6EA35E-18A5-49D8-B8EC-F6BC4CBCC004}" name="Test Case Id" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{06ABF9C3-70AE-40FC-A9C0-A75A90F2A240}" name="Test data" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{FEEB2E70-50F4-4E67-96B5-95492EACE96E}" name="Test Case Title" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{CBFF222D-2007-4326-B90F-2D4CEB89B575}" name="Pre Condition" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{685C5447-388B-49BC-AE1B-5903FE4ADEDE}" name="Steps to Execute" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{D2A3FEF5-743D-435B-AD53-E03D5CC42E81}" name="Expected Result" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{D2DBD48D-0D79-44B0-893C-8F78C6D9BEFA}" name="Actual Result" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{77F30D19-5079-4182-80EB-0B1AD53DD4C6}" name="Status" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D38A0099-B72C-4558-8215-1F794FF2115C}" name="Table8" displayName="Table8" ref="A1:J16" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:J16" xr:uid="{8465B460-5642-4945-A440-878910D61218}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{006066A9-1A00-4E3C-92C5-20DF2F4560AC}" name="Test Scenario TID"/>
+    <tableColumn id="2" xr3:uid="{B86D286F-C31F-4951-8FE0-82114A6F3CEA}" name="Test Scenario"/>
+    <tableColumn id="3" xr3:uid="{213DB056-704F-44F0-8841-D018B0708FFC}" name="Test Case Id"/>
+    <tableColumn id="4" xr3:uid="{981C1C38-B5C8-4710-BAEA-AEB28C8C0589}" name="Test data"/>
+    <tableColumn id="5" xr3:uid="{80BA245B-F08E-4A7F-95CC-E6C2F0996F17}" name="Test Case Title"/>
+    <tableColumn id="6" xr3:uid="{ACB37B6E-635B-41B0-89F1-E24B226C3106}" name="Pre Condition"/>
+    <tableColumn id="7" xr3:uid="{07801F55-5E3A-41DB-BACE-FBA112F910A1}" name="Steps to Execute"/>
+    <tableColumn id="8" xr3:uid="{103FB9A1-E086-48EA-80EE-144683B8CC3A}" name="Expected Result"/>
+    <tableColumn id="9" xr3:uid="{5932CEBA-67C1-4EBA-8D3C-9646F041E184}" name="Actual Result"/>
+    <tableColumn id="10" xr3:uid="{D8F94D5B-5304-4E2E-9072-C147C15D54B1}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -816,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A11" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,6 +1670,9 @@
       <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
@@ -955,6 +1686,9 @@
       </c>
       <c r="D14" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -1062,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726732DD-22CB-4F62-A4AF-B8D521F92FCF}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="61" zoomScaleNormal="36" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1409,12 +2143,920 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5EE776-2040-40E3-8C52-44FCC97D5826}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="109" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="79" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="89" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A76147-A5BA-4084-89B2-8EA29B2B4ABB}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="8.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BE7150-E616-4EBC-9E7B-09A7F7759072}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29C09B9-0021-4D71-B3EA-5FA6DDFE2C35}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="14"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complete testcases for overall testing
</commit_message>
<xml_diff>
--- a/01_Test_Case_Development/TestCaseDevelopment.xlsx
+++ b/01_Test_Case_Development/TestCaseDevelopment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91931\Desktop\Netflix_WebApp_Automation\01_Test_Case_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6DEB04-4E06-42DA-99AE-65127E5E2C4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68185DF-1200-4FD9-925E-A53A31D3D601}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="General Navigation TC" sheetId="5" r:id="rId5"/>
     <sheet name="PlayBack Controls Tc" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="433">
   <si>
     <t>Created By</t>
   </si>
@@ -791,6 +791,790 @@
   </si>
   <si>
     <t>TCS015</t>
+  </si>
+  <si>
+    <t>Valid movie name ('Inception')</t>
+  </si>
+  <si>
+    <t>Verify search for a valid movie</t>
+  </si>
+  <si>
+    <t>User is logged into the account</t>
+  </si>
+  <si>
+    <t>1. Enter 'Inception' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>'Inception' appears in the search results with its details.</t>
+  </si>
+  <si>
+    <t>Valid series name ('Stranger Things')</t>
+  </si>
+  <si>
+    <t>Verify search for a valid series</t>
+  </si>
+  <si>
+    <t>1. Enter 'Stranger Things' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>'Stranger Things' appears in the search results with its details.</t>
+  </si>
+  <si>
+    <t>Valid genre ('Comedy')</t>
+  </si>
+  <si>
+    <t>Verify search for a valid genre</t>
+  </si>
+  <si>
+    <t>1. Enter 'Comedy' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Movies and series under 'Comedy' appear in the search results.</t>
+  </si>
+  <si>
+    <t>Partial movie name ('Inc')</t>
+  </si>
+  <si>
+    <t>Verify search with a partial movie name</t>
+  </si>
+  <si>
+    <t>1. Enter 'Inc' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Results related to 'Inc' (e.g., 'Inception') are displayed.</t>
+  </si>
+  <si>
+    <t>Multiple keywords ('Comedy Romance')</t>
+  </si>
+  <si>
+    <t>Verify search with multiple genres</t>
+  </si>
+  <si>
+    <t>1. Enter 'Comedy Romance' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Movies and series matching 'Comedy Romance' appear in the results.</t>
+  </si>
+  <si>
+    <t>Non-alphanumeric character ('#')</t>
+  </si>
+  <si>
+    <t>Verify search with special characters</t>
+  </si>
+  <si>
+    <t>1. Enter '#' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>An appropriate message ('No results found') is displayed.</t>
+  </si>
+  <si>
+    <t>Mixed-case input ('iNcePtiOn')</t>
+  </si>
+  <si>
+    <t>Verify case-insensitive search</t>
+  </si>
+  <si>
+    <t>1. Enter 'iNcePtiOn' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Results for 'Inception' are displayed.</t>
+  </si>
+  <si>
+    <t>Valid keyword in another language ('Película')</t>
+  </si>
+  <si>
+    <t>Verify multilingual search functionality</t>
+  </si>
+  <si>
+    <t>1. Enter 'Película' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Results related to the keyword in the specified language are displayed.</t>
+  </si>
+  <si>
+    <t>Movie name with trailing spaces ('Inception ')</t>
+  </si>
+  <si>
+    <t>Verify search with trailing spaces</t>
+  </si>
+  <si>
+    <t>1. Enter 'Inception ' (with space at the end) in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Results for 'Inception' are displayed, ignoring the trailing spaces.</t>
+  </si>
+  <si>
+    <t>Valid movie/series with numbers ('Stranger Things 2')</t>
+  </si>
+  <si>
+    <t>Verify search for titles with numbers</t>
+  </si>
+  <si>
+    <t>1. Enter 'Stranger Things 2' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Results for 'Stranger Things 2' are displayed.</t>
+  </si>
+  <si>
+    <t>Invalid term ('xyz123')</t>
+  </si>
+  <si>
+    <t>Verify no results for an invalid search term</t>
+  </si>
+  <si>
+    <t>1. Enter 'xyz123' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>'No results found' message is displayed.</t>
+  </si>
+  <si>
+    <t>Empty input</t>
+  </si>
+  <si>
+    <t>Verify search with an empty input</t>
+  </si>
+  <si>
+    <t>1. Leave the search bar empty.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>'Please enter a search term' message is displayed.</t>
+  </si>
+  <si>
+    <t>Spaces only ('   ')</t>
+  </si>
+  <si>
+    <t>Verify search with only spaces</t>
+  </si>
+  <si>
+    <t>1. Enter only spaces in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>'Please enter a valid search term' message is displayed.</t>
+  </si>
+  <si>
+    <t>Long invalid string</t>
+  </si>
+  <si>
+    <t>Verify search with an excessively long invalid term</t>
+  </si>
+  <si>
+    <t>1. Enter a very long invalid term (e.g., 500+ characters).
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>SQL injection term ('1=1; DROP TABLE')</t>
+  </si>
+  <si>
+    <t>Verify handling of potential SQL injection</t>
+  </si>
+  <si>
+    <t>1. Enter '1=1; DROP TABLE' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Input is sanitized, and 'No results found' message is displayed.</t>
+  </si>
+  <si>
+    <t>Script input ('&lt;script&gt;alert('XSS')&lt;/script&gt;')</t>
+  </si>
+  <si>
+    <t>Verify handling of script injections</t>
+  </si>
+  <si>
+    <t>1. Enter '&lt;script&gt;alert('XSS')&lt;/script&gt;' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Numeric input ('12345')</t>
+  </si>
+  <si>
+    <t>Verify search with numeric-only input</t>
+  </si>
+  <si>
+    <t>1. Enter '12345' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Random symbols ('@$%&amp;*!')</t>
+  </si>
+  <si>
+    <t>Verify search with random symbols</t>
+  </si>
+  <si>
+    <t>1. Enter '@$%&amp;*!' in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>Keyword with typos ('Inceptin')</t>
+  </si>
+  <si>
+    <t>Verify results for near-matching keywords</t>
+  </si>
+  <si>
+    <t>1. Enter 'Inceptin' (typo) in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>System suggests or displays results for 'Inception.'</t>
+  </si>
+  <si>
+    <t>Unicode characters ('こんにちは')</t>
+  </si>
+  <si>
+    <t>Verify handling of Unicode characters</t>
+  </si>
+  <si>
+    <t>1. Enter 'こんにちは' (Japanese text) in the search bar.
+2. Press 'Enter.'</t>
+  </si>
+  <si>
+    <t>'No results found' message is displayed or related results appear if supported.</t>
+  </si>
+  <si>
+    <t>TCS016</t>
+  </si>
+  <si>
+    <t>TCS017</t>
+  </si>
+  <si>
+    <t>TCS018</t>
+  </si>
+  <si>
+    <t>TCS019</t>
+  </si>
+  <si>
+    <t>TCS020</t>
+  </si>
+  <si>
+    <t>TCGN001</t>
+  </si>
+  <si>
+    <t>TCGN002</t>
+  </si>
+  <si>
+    <t>TCGN003</t>
+  </si>
+  <si>
+    <t>TCGN004</t>
+  </si>
+  <si>
+    <t>TCGN005</t>
+  </si>
+  <si>
+    <t>TCGN006</t>
+  </si>
+  <si>
+    <t>TCGN007</t>
+  </si>
+  <si>
+    <t>TCGN008</t>
+  </si>
+  <si>
+    <t>TCGN009</t>
+  </si>
+  <si>
+    <t>TCGN010</t>
+  </si>
+  <si>
+    <t>TCGN011</t>
+  </si>
+  <si>
+    <t>TCGN012</t>
+  </si>
+  <si>
+    <t>TCGN013</t>
+  </si>
+  <si>
+    <t>TCGN014</t>
+  </si>
+  <si>
+    <t>TCGN015</t>
+  </si>
+  <si>
+    <t>Section: Home</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation to Home</t>
+  </si>
+  <si>
+    <t>Section: Movies</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation to Movies</t>
+  </si>
+  <si>
+    <t>Section: Series</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation to Series</t>
+  </si>
+  <si>
+    <t>Section: My List</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation to My List</t>
+  </si>
+  <si>
+    <t>Random Navigation</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation across sections</t>
+  </si>
+  <si>
+    <t>Long Navigation Test</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation for 10+ clicks</t>
+  </si>
+  <si>
+    <t>Device: Mobile</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation on mobile device</t>
+  </si>
+  <si>
+    <t>Device: Tablet</t>
+  </si>
+  <si>
+    <t>Verify smooth navigation on tablet</t>
+  </si>
+  <si>
+    <t>Movie: 'Inception'</t>
+  </si>
+  <si>
+    <t>Verify adding a movie to My List</t>
+  </si>
+  <si>
+    <t>Series: 'Stranger Things'</t>
+  </si>
+  <si>
+    <t>Verify adding a series to My List</t>
+  </si>
+  <si>
+    <t>Movie/Series already added</t>
+  </si>
+  <si>
+    <t>Verify removing a movie/series from My List</t>
+  </si>
+  <si>
+    <t>Empty My List</t>
+  </si>
+  <si>
+    <t>Verify display when My List is empty</t>
+  </si>
+  <si>
+    <t>Large My List (&gt;50 items)</t>
+  </si>
+  <si>
+    <t>Verify handling of a large number of items</t>
+  </si>
+  <si>
+    <t>Search Result: My List</t>
+  </si>
+  <si>
+    <t>Verify adding content from search to My List</t>
+  </si>
+  <si>
+    <t>Repeated Add/Remove</t>
+  </si>
+  <si>
+    <t>Verify functionality under repeated actions</t>
+  </si>
+  <si>
+    <t>Home section loads without any lag, and the content is displayed seamlessly.</t>
+  </si>
+  <si>
+    <t>Movies section loads without any lag, and the content is displayed seamlessly.</t>
+  </si>
+  <si>
+    <t>Series section loads without any lag, and the content is displayed seamlessly.</t>
+  </si>
+  <si>
+    <t>My List section loads without any lag, and the saved content is displayed correctly.</t>
+  </si>
+  <si>
+    <t>All sections load without any lag, and the navigation is seamless.</t>
+  </si>
+  <si>
+    <t>Smooth navigation is maintained without lag or app crashes.</t>
+  </si>
+  <si>
+    <t>All sections load smoothly on mobile devices without performance issues.</t>
+  </si>
+  <si>
+    <t>All sections load smoothly on tablets without performance issues.</t>
+  </si>
+  <si>
+    <t>'Inception' is added to My List, and the 'Added' confirmation is displayed.</t>
+  </si>
+  <si>
+    <t>'Stranger Things' is added to My List, and the 'Added' confirmation is displayed.</t>
+  </si>
+  <si>
+    <t>The selected movie/series is removed from My List, and the 'Removed' confirmation is displayed.</t>
+  </si>
+  <si>
+    <t>'Your list is empty' message is displayed, and the section is empty.</t>
+  </si>
+  <si>
+    <t>All items are displayed properly, and navigation remains smooth.</t>
+  </si>
+  <si>
+    <t>The selected content is successfully added to My List from the search results.</t>
+  </si>
+  <si>
+    <t>Add and remove functionality works without errors, and the list reflects the correct state consistently.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Home' in the main menu.
+2. Observe the loading time and transitions.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Movies' in the main menu.
+2. Observe the loading time and transitions.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Series' in the main menu.
+2. Observe the loading time and transitions.</t>
+  </si>
+  <si>
+    <t>1. Click on 'My List' in the main menu.
+2. Observe the loading time and transitions.</t>
+  </si>
+  <si>
+    <t>1. Navigate to each section (Home, Movies, Series, My List) randomly.
+2. Observe the loading time and transitions after each navigation.</t>
+  </si>
+  <si>
+    <t>1. Navigate across different sections repeatedly (e.g., 10 times).
+2. Observe app responsiveness after multiple navigations.</t>
+  </si>
+  <si>
+    <t>1. Open the app on a mobile device.
+2. Navigate through Home, Movies, Series, and My List.</t>
+  </si>
+  <si>
+    <t>1. Open the app on a tablet device.
+2. Navigate through Home, Movies, Series, and My List.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the Movies section.
+2. Select 'Inception.'
+3. Click 'Add to My List.'</t>
+  </si>
+  <si>
+    <t>1. Navigate to the Series section.
+2. Select 'Stranger Things.'
+3. Click 'Add to My List.'</t>
+  </si>
+  <si>
+    <t>1. Navigate to My List.
+2. Locate the movie/series already added.
+3. Click 'Remove from My List.'</t>
+  </si>
+  <si>
+    <t>1. Remove all items from My List.
+2. Navigate to My List.</t>
+  </si>
+  <si>
+    <t>1. Add 50+ movies/series to My List.
+2. Navigate to My List.
+3. Scroll through the list.</t>
+  </si>
+  <si>
+    <t>1. Search for a movie or series.
+2. Add the item from the search results to My List.
+3. Check My List.</t>
+  </si>
+  <si>
+    <t>1. Add and remove an item from My List repeatedly.
+2. Check if the list reflects the correct state each time.</t>
+  </si>
+  <si>
+    <t>Netflix Login info, Video URL</t>
+  </si>
+  <si>
+    <t>Verify Play button on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and a video is loaded</t>
+  </si>
+  <si>
+    <t>1. Open Netflix.
+2. Select a video.
+3. Click Play.</t>
+  </si>
+  <si>
+    <t>The selected video starts playing on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify Pause button on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and a video is playing</t>
+  </si>
+  <si>
+    <t>1. Start video playback on Netflix.
+2. Click Pause.</t>
+  </si>
+  <si>
+    <t>The video pauses immediately on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify Forward control on Netflix</t>
+  </si>
+  <si>
+    <t>1. Start video playback on Netflix.
+2. Use Forward control to skip ahead.</t>
+  </si>
+  <si>
+    <t>The video skips forward by the specified duration on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify Rewind control on Netflix</t>
+  </si>
+  <si>
+    <t>1. Start video playback on Netflix.
+2. Use Rewind control to go back.</t>
+  </si>
+  <si>
+    <t>The video skips backward by the specified duration on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify Volume adjustment on Netflix</t>
+  </si>
+  <si>
+    <t>1. Start video playback on Netflix.
+2. Adjust the volume slider to different levels.</t>
+  </si>
+  <si>
+    <t>The video volume changes accordingly on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify Mute control on Netflix</t>
+  </si>
+  <si>
+    <t>1. Start video playback on Netflix.
+2. Click Mute.</t>
+  </si>
+  <si>
+    <t>The video mutes and no sound is heard on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify Unmute control on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and a video is muted and playing</t>
+  </si>
+  <si>
+    <t>1. Start video playback on Netflix.
+2. Click Unmute.</t>
+  </si>
+  <si>
+    <t>The video sound resumes at the last set volume on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify seeking on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and a video is loaded/playing</t>
+  </si>
+  <si>
+    <t>1. Seek to a specific time using the timeline slider on Netflix.
+2. Verify play, pause, and volume control.</t>
+  </si>
+  <si>
+    <t>All playback controls function seamlessly during seek on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify control responsiveness on Netflix</t>
+  </si>
+  <si>
+    <t>1. Test all controls (play, pause, forward, rewind, volume) on different devices (desktop, mobile) and browsers.</t>
+  </si>
+  <si>
+    <t>Playback controls are responsive across devices and browsers on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify video start on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and video URL is valid</t>
+  </si>
+  <si>
+    <t>1. Open Netflix.
+2. Select a video.
+3. Observe the loading time and video start.</t>
+  </si>
+  <si>
+    <t>The video starts within an acceptable loading time (&lt;3 seconds) on Netflix.</t>
+  </si>
+  <si>
+    <t>Verify playback on Chrome for Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and uses Chrome browser</t>
+  </si>
+  <si>
+    <t>1. Open Netflix in Chrome.
+2. Select and play a video.</t>
+  </si>
+  <si>
+    <t>The video plays seamlessly on Netflix using Chrome.</t>
+  </si>
+  <si>
+    <t>Verify playback on Firefox for Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and uses Firefox browser</t>
+  </si>
+  <si>
+    <t>1. Open Netflix in Firefox.
+2. Select and play a video.</t>
+  </si>
+  <si>
+    <t>The video plays seamlessly on Netflix using Firefox.</t>
+  </si>
+  <si>
+    <t>Verify playback on Safari for Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and uses Safari browser</t>
+  </si>
+  <si>
+    <t>1. Open Netflix in Safari.
+2. Select and play a video.</t>
+  </si>
+  <si>
+    <t>The video plays seamlessly on Netflix using Safari.</t>
+  </si>
+  <si>
+    <t>Verify playback on mobile devices for Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix on a mobile device</t>
+  </si>
+  <si>
+    <t>1. Open Netflix on a mobile browser/app.
+2. Select and play a video.</t>
+  </si>
+  <si>
+    <t>The video plays seamlessly on Netflix on mobile devices.</t>
+  </si>
+  <si>
+    <t>Netflix Login info, Video URL, Quality=HD</t>
+  </si>
+  <si>
+    <t>Verify HD quality on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and video supports HD quality</t>
+  </si>
+  <si>
+    <t>1. Select and play a video.
+2. Switch to HD quality.</t>
+  </si>
+  <si>
+    <t>The video streams in HD quality without lag on Netflix.</t>
+  </si>
+  <si>
+    <t>Netflix Login info, Video URL, Network speed</t>
+  </si>
+  <si>
+    <t>Verify adaptive streaming on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and network connection is variable</t>
+  </si>
+  <si>
+    <t>1. Play video on Netflix using a slow network.
+2. Observe video quality auto-adjustment based on speed.</t>
+  </si>
+  <si>
+    <t>The video quality adapts seamlessly based on the network speed on Netflix.</t>
+  </si>
+  <si>
+    <t>Netflix Login info, Video URL, Subtitle file</t>
+  </si>
+  <si>
+    <t>Verify subtitles on Netflix</t>
+  </si>
+  <si>
+    <t>User is logged into Netflix and subtitle file is available</t>
+  </si>
+  <si>
+    <t>1. Select and play a video with subtitles enabled.
+2. Verify subtitle sync with the video.</t>
+  </si>
+  <si>
+    <t>Subtitles are synced with the video playback on Netflix.</t>
+  </si>
+  <si>
+    <t>TCPB001</t>
+  </si>
+  <si>
+    <t>TCPB002</t>
+  </si>
+  <si>
+    <t>TCPB003</t>
+  </si>
+  <si>
+    <t>TCPB004</t>
+  </si>
+  <si>
+    <t>TCPB005</t>
+  </si>
+  <si>
+    <t>TCPB006</t>
+  </si>
+  <si>
+    <t>TCPB007</t>
+  </si>
+  <si>
+    <t>TCPB008</t>
+  </si>
+  <si>
+    <t>TCPB009</t>
+  </si>
+  <si>
+    <t>PlayBack Controls</t>
+  </si>
+  <si>
+    <t>TCPB010</t>
+  </si>
+  <si>
+    <t>TCPB011</t>
+  </si>
+  <si>
+    <t>TCPB012</t>
+  </si>
+  <si>
+    <t>TCPB013</t>
+  </si>
+  <si>
+    <t>TCPB014</t>
+  </si>
+  <si>
+    <t>TCPB015</t>
+  </si>
+  <si>
+    <t>TCPB016</t>
+  </si>
+  <si>
+    <t>TCPB017</t>
   </si>
 </sst>
 </file>
@@ -855,7 +1639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -928,11 +1712,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -961,30 +1769,232 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="79">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1020,42 +2030,45 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1095,23 +2108,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1179,21 +2175,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C47E57B-2296-45A5-AA1A-337942628575}" name="Table2" displayName="Table2" ref="A3:B7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C47E57B-2296-45A5-AA1A-337942628575}" name="Table2" displayName="Table2" ref="A3:B7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="78">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{ED7C2092-802D-4D55-A444-B5C75D826FBF}" name="Column1" headerRowDxfId="30" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{7EA96A78-BA0E-406E-BFCA-4C90A19F9EAB}" name="Column2" headerRowDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{ED7C2092-802D-4D55-A444-B5C75D826FBF}" name="Column1" headerRowDxfId="77" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{7EA96A78-BA0E-406E-BFCA-4C90A19F9EAB}" name="Column2" headerRowDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DD051A1-F5AF-4E0C-9B05-8FE6170F8E39}" name="Table3" displayName="Table3" ref="A12:E21" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DD051A1-F5AF-4E0C-9B05-8FE6170F8E39}" name="Table3" displayName="Table3" ref="A12:E20" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{298EAB1B-CE47-48B1-B114-A849A5E4FBC3}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{57FEDC33-0ABF-4C2A-85EA-404A55DAE3A2}" name="Column2" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{7A3F631E-F0E8-4AAA-9860-670D033DF9BD}" name="Column3" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{57FEDC33-0ABF-4C2A-85EA-404A55DAE3A2}" name="Column2" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{7A3F631E-F0E8-4AAA-9860-670D033DF9BD}" name="Column3" dataDxfId="73"/>
     <tableColumn id="4" xr3:uid="{33C87811-FC0A-4F1E-906D-96F3E0410E43}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{D88CF226-9216-4B0E-9F96-5BA54F5B07B3}" name="Column5"/>
   </tableColumns>
@@ -1202,16 +2198,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6A09C3-FC34-4D8C-A5D4-8072AD62C9CC}" name="Table1" displayName="Table1" ref="A3:J12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C6A09C3-FC34-4D8C-A5D4-8072AD62C9CC}" name="Table1" displayName="Table1" ref="A3:J12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{FA4190CF-869B-4AAD-AB85-D1D406A51822}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{0311160A-A013-418B-9B3E-7E1B2ADD899B}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{AD8808FF-8F1D-4CC3-B622-EFC81FB03BD4}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{9C5B5206-F216-4894-9B82-02A62D750777}" name="Column4" headerRowDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{82A966FE-4084-4D7C-963B-761EEE522C1D}" name="Column5" headerRowDxfId="22" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{37CB4985-744D-4D93-A860-52EF4AABD929}" name="Column6" headerRowDxfId="20" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{C9BD0B30-409A-4BBC-B40E-4748725B9EDC}" name="Column7" headerRowDxfId="18" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{FD7333FE-2577-49E7-9EEB-639591C024D9}" name="Column8" headerRowDxfId="16" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{9C5B5206-F216-4894-9B82-02A62D750777}" name="Column4" headerRowDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{82A966FE-4084-4D7C-963B-761EEE522C1D}" name="Column5" headerRowDxfId="69" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{37CB4985-744D-4D93-A860-52EF4AABD929}" name="Column6" headerRowDxfId="67" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{C9BD0B30-409A-4BBC-B40E-4748725B9EDC}" name="Column7" headerRowDxfId="65" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{FD7333FE-2577-49E7-9EEB-639591C024D9}" name="Column8" headerRowDxfId="63" dataDxfId="62"/>
     <tableColumn id="9" xr3:uid="{FFBE56F5-BD1B-45B6-82E9-4F8E26DCAC44}" name="Column9"/>
     <tableColumn id="10" xr3:uid="{6A548CC8-DC51-4A5D-B5CC-BC1FD564AB3A}" name="Column10"/>
   </tableColumns>
@@ -1220,7 +2216,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{68C63221-97A0-4792-887D-F663C0F6D441}" name="Table5" displayName="Table5" ref="A1:J17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{68C63221-97A0-4792-887D-F663C0F6D441}" name="Table5" displayName="Table5" ref="A1:J17" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58">
   <autoFilter ref="A1:J17" xr:uid="{1824CCDB-4630-4D24-B722-9D28F2EBE92F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1236,22 +2232,22 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{6D6A53C9-CB2B-42B5-8A0C-459649608A20}" name="Test Scenario TID"/>
     <tableColumn id="2" xr3:uid="{2062CCCD-C2CB-4254-A6CC-757B0FC707B8}" name="Test Scenario"/>
-    <tableColumn id="3" xr3:uid="{8F6EA35E-18A5-49D8-B8EC-F6BC4CBCC004}" name="Test Case Id" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{06ABF9C3-70AE-40FC-A9C0-A75A90F2A240}" name="Test data" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{FEEB2E70-50F4-4E67-96B5-95492EACE96E}" name="Test Case Title" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{CBFF222D-2007-4326-B90F-2D4CEB89B575}" name="Pre Condition" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{685C5447-388B-49BC-AE1B-5903FE4ADEDE}" name="Steps to Execute" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{D2A3FEF5-743D-435B-AD53-E03D5CC42E81}" name="Expected Result" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{D2DBD48D-0D79-44B0-893C-8F78C6D9BEFA}" name="Actual Result" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{77F30D19-5079-4182-80EB-0B1AD53DD4C6}" name="Status" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{8F6EA35E-18A5-49D8-B8EC-F6BC4CBCC004}" name="Test Case Id" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{06ABF9C3-70AE-40FC-A9C0-A75A90F2A240}" name="Test data" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{FEEB2E70-50F4-4E67-96B5-95492EACE96E}" name="Test Case Title" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{CBFF222D-2007-4326-B90F-2D4CEB89B575}" name="Pre Condition" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{685C5447-388B-49BC-AE1B-5903FE4ADEDE}" name="Steps to Execute" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{D2A3FEF5-743D-435B-AD53-E03D5CC42E81}" name="Expected Result" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{D2DBD48D-0D79-44B0-893C-8F78C6D9BEFA}" name="Actual Result" dataDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{77F30D19-5079-4182-80EB-0B1AD53DD4C6}" name="Status" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D38A0099-B72C-4558-8215-1F794FF2115C}" name="Table8" displayName="Table8" ref="A1:J16" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:J16" xr:uid="{8465B460-5642-4945-A440-878910D61218}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D38A0099-B72C-4558-8215-1F794FF2115C}" name="Table8" displayName="Table8" ref="A1:J21" totalsRowShown="0" headerRowDxfId="49" dataDxfId="36" headerRowBorderDxfId="48" tableBorderDxfId="47">
+  <autoFilter ref="A1:J21" xr:uid="{8465B460-5642-4945-A440-878910D61218}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1264,16 +2260,64 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{006066A9-1A00-4E3C-92C5-20DF2F4560AC}" name="Test Scenario TID"/>
-    <tableColumn id="2" xr3:uid="{B86D286F-C31F-4951-8FE0-82114A6F3CEA}" name="Test Scenario"/>
-    <tableColumn id="3" xr3:uid="{213DB056-704F-44F0-8841-D018B0708FFC}" name="Test Case Id"/>
-    <tableColumn id="4" xr3:uid="{981C1C38-B5C8-4710-BAEA-AEB28C8C0589}" name="Test data"/>
-    <tableColumn id="5" xr3:uid="{80BA245B-F08E-4A7F-95CC-E6C2F0996F17}" name="Test Case Title"/>
-    <tableColumn id="6" xr3:uid="{ACB37B6E-635B-41B0-89F1-E24B226C3106}" name="Pre Condition"/>
-    <tableColumn id="7" xr3:uid="{07801F55-5E3A-41DB-BACE-FBA112F910A1}" name="Steps to Execute"/>
-    <tableColumn id="8" xr3:uid="{103FB9A1-E086-48EA-80EE-144683B8CC3A}" name="Expected Result"/>
-    <tableColumn id="9" xr3:uid="{5932CEBA-67C1-4EBA-8D3C-9646F041E184}" name="Actual Result"/>
-    <tableColumn id="10" xr3:uid="{D8F94D5B-5304-4E2E-9072-C147C15D54B1}" name="Status"/>
+    <tableColumn id="1" xr3:uid="{006066A9-1A00-4E3C-92C5-20DF2F4560AC}" name="Test Scenario TID" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{B86D286F-C31F-4951-8FE0-82114A6F3CEA}" name="Test Scenario" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{213DB056-704F-44F0-8841-D018B0708FFC}" name="Test Case Id" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{981C1C38-B5C8-4710-BAEA-AEB28C8C0589}" name="Test data" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{80BA245B-F08E-4A7F-95CC-E6C2F0996F17}" name="Test Case Title" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{ACB37B6E-635B-41B0-89F1-E24B226C3106}" name="Pre Condition" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{07801F55-5E3A-41DB-BACE-FBA112F910A1}" name="Steps to Execute" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{103FB9A1-E086-48EA-80EE-144683B8CC3A}" name="Expected Result" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{5932CEBA-67C1-4EBA-8D3C-9646F041E184}" name="Actual Result" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{D8F94D5B-5304-4E2E-9072-C147C15D54B1}" name="Status" dataDxfId="37"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D7D6B60F-CF13-4B7F-B1CA-96A73EBBD28C}" name="Table7" displayName="Table7" ref="A2:J16" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="35">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{41B8F590-2CC3-4CC4-858D-0F4769FF4897}" name="Column1" headerRowDxfId="25" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{EFB59916-0A64-4785-A703-F48721260C1E}" name="Column2" headerRowDxfId="26" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{0754E69D-A9CA-423E-A2EC-927F77F33AA1}" name="Column3" headerRowDxfId="27" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{7EE27E11-59CE-402A-88E1-E661328B4612}" name="Column4" headerRowDxfId="28" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{715C041E-9B0F-4664-AB9D-FE50101B181A}" name="Column5" headerRowDxfId="29" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{AE102C56-136B-45D8-8936-C41A450051D4}" name="Column6" headerRowDxfId="30" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{247DA2E4-80E5-4F76-A3F1-C4E86E16AD85}" name="Column7" headerRowDxfId="31" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{A0912B6C-2BCF-4513-A2C6-52054CF20231}" name="Column8" headerRowDxfId="32" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{97B1B697-F715-4C51-BA2B-4F25B9DA61A5}" name="Column9" headerRowDxfId="33" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{44E50922-2575-4EAB-8C5A-1579AD60FA9D}" name="Column10" headerRowDxfId="34" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{349B4269-E2A0-42BB-B70C-0593F0A60523}" name="Table9" displayName="Table9" ref="A1:J18" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="12">
+  <autoFilter ref="A1:J18" xr:uid="{984BEEDA-7470-4040-A79F-C9C3A840A129}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{7E1E6333-C724-44A3-9D56-128751DDBCE3}" name="Test Scenario TID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{BD14DE3D-832F-4A4A-8C8A-129DBC8DB050}" name="Test Scenario" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{5EDCD5ED-C583-4987-92D8-0D9871815F76}" name="Test Case Id" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{CC5104BC-F693-4765-AFEE-F52F09F375A0}" name="Test data" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{D05BD8E9-F23E-4E49-A9A0-3219FC9AB4AF}" name="Test Case Title" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{5E86352A-292D-4E7C-A1C2-0F23B0AFD20E}" name="Pre Condition" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{399CB9A9-ED48-4859-87AB-053E2BAAE239}" name="Steps to Execute" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{FA3E35A0-2AA7-4A35-A60E-808D46BE6123}" name="Expected Result" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{95902C92-1495-4603-9339-83703F0568E3}" name="Actual Result" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{8636D5DE-B012-43C8-A9AD-8E6EF37C05A8}" name="Status" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1544,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="99" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1559,10 +2603,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1704,6 +2748,9 @@
       <c r="D15" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
@@ -1718,8 +2765,11 @@
       <c r="D16" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
@@ -1732,8 +2782,11 @@
       <c r="D17" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -1746,8 +2799,11 @@
       <c r="D18" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
@@ -1760,8 +2816,11 @@
       <c r="D19" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>35</v>
       </c>
@@ -1774,8 +2833,11 @@
       <c r="D20" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
     </row>
@@ -1797,7 +2859,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScale="61" zoomScaleNormal="36" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1809,7 +2871,7 @@
     <col min="5" max="5" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.08984375" customWidth="1"/>
     <col min="7" max="7" width="21.1796875" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
     <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.1796875" customWidth="1"/>
   </cols>
@@ -1846,7 +2908,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1872,7 +2934,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1898,7 +2960,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1924,7 +2986,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1950,7 +3012,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1976,7 +3038,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2002,7 +3064,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2054,7 +3116,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2080,7 +3142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2106,7 +3168,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2145,8 +3207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5EE776-2040-40E3-8C52-44FCC97D5826}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="86" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2154,47 +3216,47 @@
     <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
     <col min="5" max="5" width="14.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" customWidth="1"/>
+    <col min="7" max="7" width="41.7265625" customWidth="1"/>
+    <col min="8" max="8" width="25.6328125" customWidth="1"/>
     <col min="9" max="9" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -2223,7 +3285,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -2252,7 +3314,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -2280,7 +3342,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -2308,7 +3370,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
@@ -2336,7 +3398,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2364,7 +3426,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="79" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -2392,7 +3454,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="89" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
@@ -2448,7 +3510,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -2476,7 +3538,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -2504,7 +3566,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -2532,7 +3594,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
@@ -2560,7 +3622,7 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
@@ -2588,7 +3650,7 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
@@ -2616,7 +3678,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
@@ -2667,10 +3729,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A76147-A5BA-4084-89B2-8EA29B2B4ABB}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="76" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2678,218 +3740,606 @@
     <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.90625" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="46.08984375" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="33.7265625" customWidth="1"/>
+    <col min="8" max="8" width="34.08984375" customWidth="1"/>
     <col min="9" max="9" width="13.7265625" customWidth="1"/>
     <col min="10" max="10" width="8.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="D2" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="D3" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="12" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D4" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="D5" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="D6" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="D7" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="12" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="D8" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="D9" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="12" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="D10" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="16" t="s">
+      <c r="D11" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="12" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D12" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="16" t="s">
+      <c r="D13" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="12" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D14" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="D15" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" t="s">
         <v>190</v>
       </c>
+      <c r="D16" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>268</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>272</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2901,13 +4351,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BE7150-E616-4EBC-9E7B-09A7F7759072}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
+    <sheetView topLeftCell="A15" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="12" style="11" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.08984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.54296875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="52.81640625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" style="11"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
@@ -2941,122 +4404,986 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="145" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="14"/>
+    <row r="2" spans="1:10" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29C09B9-0021-4D71-B3EA-5FA6DDFE2C35}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="28.26953125" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="8.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="86.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="14"/>
+    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>